<commit_message>
Fix errors in graphics dimensions
</commit_message>
<xml_diff>
--- a/app/webroot/angular/references/amd_stats_datas.xlsx
+++ b/app/webroot/angular/references/amd_stats_datas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8595" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8595" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="height based old" sheetId="1" r:id="rId1"/>
@@ -4951,7 +4951,7 @@
   <dimension ref="A1:AG30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9456,8 +9456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9524,9 +9524,8 @@
       <c r="I2">
         <v>89</v>
       </c>
-      <c r="J2" t="str">
-        <f>IF('age based'!J2&gt;0,"[" &amp; 'age based'!J$1&amp; "," &amp; SUBSTITUTE(TEXT('age based'!J2,"#0,#"),",",".")&amp;"] ,","")&amp;K2</f>
-        <v>0</v>
+      <c r="J2">
+        <v>2</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -10068,8 +10067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10118,7 +10117,7 @@
       </c>
       <c r="J2" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A2&amp;"."&amp;dimensions!J$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!J2,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_m.vbottom=0.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_m.vbottom=2.;</v>
       </c>
       <c r="K2" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A2&amp;"."&amp;dimensions!K$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!K2,"#0,###"),",",".")&amp;";"</f>

</xml_diff>

<commit_message>
Sex = null -> sex = "u"
</commit_message>
<xml_diff>
--- a/app/webroot/angular/references/amd_stats_datas.xlsx
+++ b/app/webroot/angular/references/amd_stats_datas.xlsx
@@ -213,10 +213,10 @@
     <t>bmi</t>
   </si>
   <si>
-    <t>null</t>
+    <t>Weightkg</t>
   </si>
   <si>
-    <t>Weightkg</t>
+    <t>u</t>
   </si>
 </sst>
 </file>
@@ -9457,7 +9457,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9504,7 +9504,7 @@
         <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -9584,7 +9584,7 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>ageAtConsultTime_Weightkg_null</v>
+        <v>ageAtConsultTime_Weightkg_u</v>
       </c>
       <c r="B4" t="str">
         <f>B3</f>
@@ -9595,7 +9595,7 @@
         <v>Weightkg</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E7" si="2">E3</f>
@@ -9727,7 +9727,7 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>ageAtConsultTime_Heightcm_null</v>
+        <v>ageAtConsultTime_Heightcm_u</v>
       </c>
       <c r="B7" t="str">
         <f>B6</f>
@@ -9739,7 +9739,7 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="6"/>
-        <v>null</v>
+        <v>u</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
@@ -9783,7 +9783,7 @@
         <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="6"/>
@@ -9869,7 +9869,7 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>Heightcm_Weightkg_null</v>
+        <v>Heightcm_Weightkg_u</v>
       </c>
       <c r="B10" t="str">
         <f>B9</f>
@@ -9881,7 +9881,7 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="6"/>
-        <v>null</v>
+        <v>u</v>
       </c>
       <c r="E10">
         <f t="shared" si="7"/>
@@ -10011,7 +10011,7 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>ageAtConsultTime_bmi_null</v>
+        <v>ageAtConsultTime_bmi_u</v>
       </c>
       <c r="B13" t="str">
         <f>B12</f>
@@ -10023,7 +10023,7 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="6"/>
-        <v>null</v>
+        <v>u</v>
       </c>
       <c r="E13">
         <f t="shared" si="7"/>
@@ -10169,39 +10169,39 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"={};"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null={};</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u={};</v>
       </c>
       <c r="E4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!E$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!E4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.top=0.05;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.top=0.05;</v>
       </c>
       <c r="F4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!F$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!F4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.bottom=0.95;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.bottom=0.95;</v>
       </c>
       <c r="G4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!G$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!G4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.left=0.03;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.left=0.03;</v>
       </c>
       <c r="H4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!H$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!H4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.right=0.97;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.right=0.97;</v>
       </c>
       <c r="I4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!I$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!I4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.vtop=89.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.vtop=89.;</v>
       </c>
       <c r="J4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!J$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!J4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.vbottom=2.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.vbottom=2.;</v>
       </c>
       <c r="K4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!K$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!K4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.vleft=0.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.vleft=0.;</v>
       </c>
       <c r="L4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!L$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!L4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.vright=20.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.vright=20.;</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -10283,39 +10283,39 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"={};"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null={};</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u={};</v>
       </c>
       <c r="E7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!E$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!E7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.top=0.05;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.top=0.05;</v>
       </c>
       <c r="F7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!F$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!F7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.bottom=0.95;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.bottom=0.95;</v>
       </c>
       <c r="G7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!G$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!G7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.left=0.03;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.left=0.03;</v>
       </c>
       <c r="H7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!H$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!H7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.right=0.97;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.right=0.97;</v>
       </c>
       <c r="I7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!I$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!I7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.vtop=186.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.vtop=186.;</v>
       </c>
       <c r="J7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!J$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!J7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.vbottom=46.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.vbottom=46.;</v>
       </c>
       <c r="K7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!K$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!K7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.vleft=0.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.vleft=0.;</v>
       </c>
       <c r="L7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!L$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!L7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.vright=20.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.vright=20.;</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -10397,39 +10397,39 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"={};"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_null={};</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_u={};</v>
       </c>
       <c r="E10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!E$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!E10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_null.top=0.05;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_u.top=0.05;</v>
       </c>
       <c r="F10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!F$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!F10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_null.bottom=0.95;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_u.bottom=0.95;</v>
       </c>
       <c r="G10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!G$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!G10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_null.left=0.03;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_u.left=0.03;</v>
       </c>
       <c r="H10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!H$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!H10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_null.right=0.97;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_u.right=0.97;</v>
       </c>
       <c r="I10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!I$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!I10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_null.vtop=26.;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_u.vtop=26.;</v>
       </c>
       <c r="J10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!J$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!J10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_null.vbottom=9.;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_u.vbottom=9.;</v>
       </c>
       <c r="K10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!K$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!K10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_null.vleft=80.;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_u.vleft=80.;</v>
       </c>
       <c r="L10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!L$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!L10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_null.vright=120.;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_u.vright=120.;</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -10511,39 +10511,39 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"={};"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null={};</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u={};</v>
       </c>
       <c r="E13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!E$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!E13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.top=0.05;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.top=0.05;</v>
       </c>
       <c r="F13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!F$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!F13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.bottom=0.95;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.bottom=0.95;</v>
       </c>
       <c r="G13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!G$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!G13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.left=0.03;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.left=0.03;</v>
       </c>
       <c r="H13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!H$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!H13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.right=0.97;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.right=0.97;</v>
       </c>
       <c r="I13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!I$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!I13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.vtop=31.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.vtop=31.;</v>
       </c>
       <c r="J13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!J$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!J13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.vbottom=13.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.vbottom=13.;</v>
       </c>
       <c r="K13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!K$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!K13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.vleft=2.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.vleft=2.;</v>
       </c>
       <c r="L13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!L$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!L13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.vright=20.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.vright=20.;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Sex = null -> sex = "u""
This reverts commit b5fefc9685b82eeb6e1e4235372e86358ec51ee6.
</commit_message>
<xml_diff>
--- a/app/webroot/angular/references/amd_stats_datas.xlsx
+++ b/app/webroot/angular/references/amd_stats_datas.xlsx
@@ -213,10 +213,10 @@
     <t>bmi</t>
   </si>
   <si>
-    <t>Weightkg</t>
+    <t>null</t>
   </si>
   <si>
-    <t>u</t>
+    <t>Weightkg</t>
   </si>
 </sst>
 </file>
@@ -9457,7 +9457,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9504,7 +9504,7 @@
         <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -9584,7 +9584,7 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>ageAtConsultTime_Weightkg_u</v>
+        <v>ageAtConsultTime_Weightkg_null</v>
       </c>
       <c r="B4" t="str">
         <f>B3</f>
@@ -9595,7 +9595,7 @@
         <v>Weightkg</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E7" si="2">E3</f>
@@ -9727,7 +9727,7 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>ageAtConsultTime_Heightcm_u</v>
+        <v>ageAtConsultTime_Heightcm_null</v>
       </c>
       <c r="B7" t="str">
         <f>B6</f>
@@ -9739,7 +9739,7 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="6"/>
-        <v>u</v>
+        <v>null</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
@@ -9783,7 +9783,7 @@
         <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="6"/>
@@ -9869,7 +9869,7 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>Heightcm_Weightkg_u</v>
+        <v>Heightcm_Weightkg_null</v>
       </c>
       <c r="B10" t="str">
         <f>B9</f>
@@ -9881,7 +9881,7 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="6"/>
-        <v>u</v>
+        <v>null</v>
       </c>
       <c r="E10">
         <f t="shared" si="7"/>
@@ -10011,7 +10011,7 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>ageAtConsultTime_bmi_u</v>
+        <v>ageAtConsultTime_bmi_null</v>
       </c>
       <c r="B13" t="str">
         <f>B12</f>
@@ -10023,7 +10023,7 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="6"/>
-        <v>u</v>
+        <v>null</v>
       </c>
       <c r="E13">
         <f t="shared" si="7"/>
@@ -10169,39 +10169,39 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"={};"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u={};</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null={};</v>
       </c>
       <c r="E4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!E$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!E4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.top=0.05;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.top=0.05;</v>
       </c>
       <c r="F4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!F$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!F4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.bottom=0.95;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.bottom=0.95;</v>
       </c>
       <c r="G4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!G$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!G4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.left=0.03;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.left=0.03;</v>
       </c>
       <c r="H4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!H$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!H4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.right=0.97;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.right=0.97;</v>
       </c>
       <c r="I4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!I$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!I4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.vtop=89.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.vtop=89.;</v>
       </c>
       <c r="J4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!J$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!J4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.vbottom=2.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.vbottom=2.;</v>
       </c>
       <c r="K4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!K$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!K4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.vleft=0.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.vleft=0.;</v>
       </c>
       <c r="L4" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A4&amp;"."&amp;dimensions!L$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!L4,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_u.vright=20.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Weightkg_null.vright=20.;</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -10283,39 +10283,39 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"={};"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u={};</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null={};</v>
       </c>
       <c r="E7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!E$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!E7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.top=0.05;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.top=0.05;</v>
       </c>
       <c r="F7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!F$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!F7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.bottom=0.95;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.bottom=0.95;</v>
       </c>
       <c r="G7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!G$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!G7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.left=0.03;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.left=0.03;</v>
       </c>
       <c r="H7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!H$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!H7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.right=0.97;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.right=0.97;</v>
       </c>
       <c r="I7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!I$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!I7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.vtop=186.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.vtop=186.;</v>
       </c>
       <c r="J7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!J$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!J7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.vbottom=46.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.vbottom=46.;</v>
       </c>
       <c r="K7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!K$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!K7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.vleft=0.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.vleft=0.;</v>
       </c>
       <c r="L7" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A7&amp;"."&amp;dimensions!L$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!L7,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_u.vright=20.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_Heightcm_null.vright=20.;</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -10397,39 +10397,39 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"={};"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_u={};</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_null={};</v>
       </c>
       <c r="E10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!E$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!E10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_u.top=0.05;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_null.top=0.05;</v>
       </c>
       <c r="F10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!F$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!F10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_u.bottom=0.95;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_null.bottom=0.95;</v>
       </c>
       <c r="G10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!G$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!G10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_u.left=0.03;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_null.left=0.03;</v>
       </c>
       <c r="H10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!H$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!H10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_u.right=0.97;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_null.right=0.97;</v>
       </c>
       <c r="I10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!I$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!I10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_u.vtop=26.;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_null.vtop=26.;</v>
       </c>
       <c r="J10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!J$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!J10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_u.vbottom=9.;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_null.vbottom=9.;</v>
       </c>
       <c r="K10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!K$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!K10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_u.vleft=80.;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_null.vleft=80.;</v>
       </c>
       <c r="L10" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A10&amp;"."&amp;dimensions!L$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!L10,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.Heightcm_Weightkg_u.vright=120.;</v>
+        <v>amd_stats.dimensions.Heightcm_Weightkg_null.vright=120.;</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -10511,39 +10511,39 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"={};"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u={};</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null={};</v>
       </c>
       <c r="E13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!E$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!E13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.top=0.05;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.top=0.05;</v>
       </c>
       <c r="F13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!F$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!F13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.bottom=0.95;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.bottom=0.95;</v>
       </c>
       <c r="G13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!G$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!G13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.left=0.03;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.left=0.03;</v>
       </c>
       <c r="H13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!H$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!H13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.right=0.97;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.right=0.97;</v>
       </c>
       <c r="I13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!I$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!I13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.vtop=31.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.vtop=31.;</v>
       </c>
       <c r="J13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!J$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!J13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.vbottom=13.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.vbottom=13.;</v>
       </c>
       <c r="K13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!K$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!K13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.vleft=2.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.vleft=2.;</v>
       </c>
       <c r="L13" t="str">
         <f>dimensions!$A$1&amp;"."&amp;dimensions!$A13&amp;"."&amp;dimensions!L$1&amp;"="&amp; SUBSTITUTE(TEXT(dimensions!L13,"#0,###"),",",".")&amp;";"</f>
-        <v>amd_stats.dimensions.ageAtConsultTime_bmi_u.vright=20.;</v>
+        <v>amd_stats.dimensions.ageAtConsultTime_bmi_null.vright=20.;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>